<commit_message>
Spiced up boss fight and squashed bugs
</commit_message>
<xml_diff>
--- a/1DAE21_Belmans_Jef_CaveCrawler/Belmans_Jef_CaveCrawler/Resources/Belmans_Jef_Game.xlsx
+++ b/1DAE21_Belmans_Jef_CaveCrawler/Belmans_Jef_CaveCrawler/Resources/Belmans_Jef_Game.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25310"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25409"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2019_2020\_Programming2\00_GameProject\ForStudents\Description&amp;Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{397E21C5-16C0-4325-8387-6A040C063B22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{076231E2-6DB6-4469-BDA1-1628A75264EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8472" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8472" firstSheet="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Basic Game rubric" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>Game</t>
   </si>
@@ -63,31 +63,31 @@
     <t>Animations</t>
   </si>
   <si>
-    <t>Multiple enviromental hazards are animated. one hazard (a hand) has contact animations. Cannon that aims it barrel at the player as he moves. Upon taking damage the sprite flashes red.</t>
+    <t>Multiple enviromental hazards are animated. one hazard (a hand) has contact animations. Cannon that aims it barrel at the player as he moves. Boss that has a charge, jump and land animation. Upon taking damage the sprite flashes red. When the player / enemy dies, a procedural particle system is played.</t>
   </si>
   <si>
     <t>Interactions</t>
   </si>
   <si>
-    <t>Almost all hazards can be killed / destroyed using the player gun that shoots projectiles which damage and kill said hazards</t>
+    <t>Almost all hazards can be killed / destroyed using the player gun that shoots projectiles which damage and kill said hazards. There are hazards that drop from the ceiling and damage the player on contact, hazards that rise from the ground whem the player gets close, cannons that aim and shoot at the player when in sight, a boss that jumps and shoots towards the player.</t>
   </si>
   <si>
     <t>Game implementation</t>
   </si>
   <si>
-    <t>At the moment there are 9 different gameobjects the player can interact with in different ways (shooting them, walking over/on them, walking past them)</t>
+    <t>At the moment there are more than 10 different gameobjects the player can interact with in different ways (shooting them, walking over/on them, walking past them, walking in sight)</t>
   </si>
   <si>
     <t>HUD and UI</t>
   </si>
   <si>
-    <t>Basic health UI implemented. Implemented following menus: main menu with link to options menu and quit button, options menu to adjust volume, pause menu that freezes the game and can restart / go back to menu. end of level screen to restart / go back to menu</t>
+    <t>Health and score UI implemented. Implemented following menus: main menu with link to options menu and quit button, options menu to adjust volume, pause menu that freezes the game and can restart / go back to menu. end of level screen to go to the next level/ back to menu. End of game screen that shows the saved highscore and current score, button to go back to menu.</t>
   </si>
   <si>
     <t>Sound</t>
   </si>
   <si>
-    <t>All actions have sound, the master volume can be adjusted using the up and down key and in the options menu.</t>
+    <t>All actions have sound, there is a main soundtrack and a boss soundtrack when starting the boss encounter. The master volume can be adjusted using the up and down buttons and in the options menu.</t>
   </si>
   <si>
     <t>Extras</t>
@@ -98,37 +98,28 @@
 </t>
   </si>
   <si>
-    <t>Animation system based on data from a file</t>
-  </si>
-  <si>
     <t>Load/save game system</t>
   </si>
   <si>
+    <t>The highscore gets loaded from a save file and displayed at the end game screen. When the player beats the previous highscore, it gets saved to a txt file.</t>
+  </si>
+  <si>
     <t>Load level from a file</t>
   </si>
   <si>
-    <t>Bone animation</t>
-  </si>
-  <si>
-    <t>Pathfinding</t>
+    <t>The level and hazards get loaded from an SVG file. all other objects (enemies, rising hands, falling spikes,..) get loaded from a custom txt file containing their properties like position, health and size.</t>
   </si>
   <si>
     <t>A.I.</t>
   </si>
   <si>
-    <t>Inventory system.</t>
-  </si>
-  <si>
-    <t>Level editor</t>
+    <t>Simple canon AI that aims its barrel towards the player and shoots when they are in sight and in range. Boss AI that charges and jumps towards the player at an interval, boss has a barrel like the cannon that aims at the player and shoots with an interval.</t>
   </si>
   <si>
     <t>Particle system</t>
   </si>
   <si>
-    <t>Level generation</t>
-  </si>
-  <si>
-    <t>…</t>
+    <t>Entirely procedural, object based particle system. Particles get pooled at compile time to save CPU usage and prevent particles from getting destroy / instanciated everytime a particle system is used.</t>
   </si>
   <si>
     <t>Screenshake</t>
@@ -137,19 +128,10 @@
     <t>Added instead of parallax, as recommended by Tom.</t>
   </si>
   <si>
-    <t>Framestats &amp; frame limiter</t>
-  </si>
-  <si>
-    <t>Framestats get printed every second to the console. The FPS can be capped to test physics performance at lower framerates.</t>
-  </si>
-  <si>
     <t>Object pooling</t>
   </si>
   <si>
-    <t>Object pooling is used to instanciate a pool of projectiles at the beginning to prevent a projectile being instanciated / destoryed everytime the player shoots</t>
-  </si>
-  <si>
-    <t>The level and hazards get loaded from an SVG file. all other objects (enemies, rising hands, falling spikes,..) get loaded from a custom txt file.</t>
+    <t>Object pooling is used to instanciate a pool of projectiles and particles at the beginning to prevent a projectile being instanciated / destoryed everytime the player shoots or a particle system plays</t>
   </si>
 </sst>
 </file>
@@ -549,9 +531,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="C7" sqref="C7"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
     </sheetView>
@@ -560,7 +542,7 @@
   <cols>
     <col min="1" max="1" width="35.28515625" customWidth="1"/>
     <col min="2" max="2" width="25.42578125" customWidth="1"/>
-    <col min="3" max="3" width="185.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="365.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="97.5">
@@ -660,9 +642,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="A17" sqref="A17"/>
+      <selection pane="bottomRight" activeCell="C13" sqref="C13"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
     </sheetView>
@@ -671,7 +653,7 @@
   <cols>
     <col min="1" max="1" width="57.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.42578125" customWidth="1"/>
-    <col min="3" max="3" width="134" customWidth="1"/>
+    <col min="3" max="3" width="228.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="46.9" customHeight="1">
@@ -690,133 +672,75 @@
         <v>17</v>
       </c>
       <c r="B2" s="1">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="16.149999999999999">
       <c r="A3" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B3" s="1">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="16.149999999999999">
       <c r="A4" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B4" s="1">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="16.149999999999999">
       <c r="A5" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B5" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="16.149999999999999">
-      <c r="A6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="16.149999999999999">
-      <c r="A7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="16.149999999999999">
-      <c r="A8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="16.149999999999999">
-      <c r="A9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="16.149999999999999">
-      <c r="A10" s="2" t="s">
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="16.149999999999999">
-      <c r="A11" s="2" t="s">
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="16.149999999999999">
-      <c r="A12" s="2" t="s">
+    </row>
+    <row r="7" spans="1:3" ht="15">
+      <c r="A7" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
         <v>28</v>
       </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="15">
-      <c r="A15" t="s">
-        <v>32</v>
-      </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="C15" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16" t="s">
-        <v>34</v>
-      </c>
-    </row>
+    </row>
+    <row r="8" spans="1:3" ht="15"/>
+    <row r="9" spans="1:3" ht="15"/>
+    <row r="11" spans="1:3" ht="15"/>
+    <row r="12" spans="1:3" ht="15"/>
+    <row r="13" spans="1:3" ht="15"/>
+    <row r="14" spans="1:3" ht="15"/>
+    <row r="15" spans="1:3" ht="15"/>
+    <row r="16" spans="1:3" ht="15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -836,15 +760,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100723942CCEB3A674D8F1F6472CCEFB38E" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b456a193ed59fb7b1c8994f62cf0bc67">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="128482ec-0431-40d5-ab26-89ea2a4f3ccd" xmlns:ns3="60eb0cf4-ae2a-4762-800a-cb593b869ecb" xmlns:ns4="http://schemas.microsoft.com/sharepoint/v4" xmlns:ns5="a2e691a9-fcfc-4d85-a390-1894fe98bd9e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a253e5da7d9e3ac9660eca9ce8fbd104" ns2:_="" ns3:_="" ns4:_="" ns5:_="">
     <xsd:import namespace="128482ec-0431-40d5-ab26-89ea2a4f3ccd"/>
@@ -1097,14 +1012,23 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B0CCE84-996D-4970-9B0F-6A269E60B9CF}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DBBEFD80-C66F-4B0C-9ED1-734A448E3DFF}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E48979D-1BFD-4ABF-A49B-E2BDAD7A21BF}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DBBEFD80-C66F-4B0C-9ED1-734A448E3DFF}"/>
 </file>
</xml_diff>